<commit_message>
Kedelai Kering - Path analysis code update
</commit_message>
<xml_diff>
--- a/R/archive/Kedelai Kering/Contoh Data Total.xlsx
+++ b/R/archive/Kedelai Kering/Contoh Data Total.xlsx
@@ -1,16 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
-  <workbookPr/>
-  <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
-  </bookViews>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -133,11 +150,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -146,19 +165,13 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri Light"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -171,14 +184,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -190,58 +196,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -250,34 +230,34 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -291,71 +271,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -379,53 +359,50 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -435,7 +412,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -444,7 +421,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -453,7 +430,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -461,10 +438,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -493,7 +470,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -506,12 +483,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -523,3011 +501,3051 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="1">
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0" showGridLines="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="7.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="6.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="12" width="6.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="12" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="12" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="12" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="12" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="12" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="12" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="12" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="13" width="6.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="12" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="12" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="12" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="12" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="12" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="12" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="12" width="8.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.125" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="2" max="2" width="12.125" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="3" max="3" width="6.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="4" max="4" width="7.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="5" max="5" width="7.75" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="6" max="6" width="7.75" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="7" max="7" width="5.75" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="8" max="8" width="7.125" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="9" max="9" width="7.25" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="10" max="10" width="5.75" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="11" max="11" width="7.75" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="12" max="12" width="7.75" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="13" max="13" width="8.375" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="14" max="14" width="7.625" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="15" max="15" width="8.125" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="16" max="16" width="8.375" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="17" max="17" width="8.125" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="18" max="18" width="9.125" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="19" max="19" width="5.75" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="20" max="20" width="9.25" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="21" max="21" width="8" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="22" max="22" width="9.375" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="23" max="23" width="7.125" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="24" max="24" width="7.5" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="25" max="25" width="7.125" customWidth="1" level="0" outlineLevel="0"/>
+    <col min="26" max="26" width="7.25" customWidth="1" level="0" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="4">
         <v>71.25</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="4">
         <v>2.5</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="4">
         <v>5.45</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="4">
         <v>5.5</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="5">
         <v>2</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="4">
         <v>2.5</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="5">
         <v>10</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="4">
         <v>2.75</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="5">
         <v>21</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="4">
         <v>5.91</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="4">
         <v>33.25</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="4">
         <v>25</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="4">
         <v>561.55</v>
       </c>
-      <c r="P2" s="7">
+      <c r="P2" s="4">
         <v>41.21</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="Q2" s="4">
         <v>9.34</v>
       </c>
-      <c r="R2" s="7">
+      <c r="R2" s="4">
         <v>5.35</v>
       </c>
-      <c r="S2" s="9">
+      <c r="S2" s="6">
         <v>3.05</v>
       </c>
-      <c r="T2" s="7">
+      <c r="T2" s="4">
         <v>91.5</v>
       </c>
-      <c r="U2" s="7">
+      <c r="U2" s="4">
         <v>25.55</v>
       </c>
-      <c r="V2" s="7">
+      <c r="V2" s="4">
         <v>290.27000000000004</v>
       </c>
-      <c r="W2" s="7">
+      <c r="W2" s="4">
         <v>6.9</v>
       </c>
-      <c r="X2" s="7">
+      <c r="X2" s="4">
         <v>6.11</v>
       </c>
-      <c r="Y2" s="7">
+      <c r="Y2" s="4">
         <v>5.38</v>
       </c>
-      <c r="Z2" s="7">
+      <c r="Z2" s="4">
         <v>17.52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="4">
         <v>74.5</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="4">
         <v>2.5</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="4">
         <v>5.275</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="4">
         <v>4.25</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="4">
         <v>1.75</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="4">
         <v>2.25</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="4">
         <v>8.25</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="4">
         <v>2.25</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="5">
         <v>20</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="4">
         <v>5.44</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="5">
         <v>31</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="4">
         <v>31.5</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="4">
         <v>687.95</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="4">
         <v>40.23</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="4">
         <v>7.91</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3" s="4">
         <v>5.19</v>
       </c>
-      <c r="S3" s="9">
+      <c r="S3" s="6">
         <v>2.93</v>
       </c>
-      <c r="T3" s="7">
+      <c r="T3" s="4">
         <v>84.5</v>
       </c>
-      <c r="U3" s="7">
+      <c r="U3" s="4">
         <v>28.26</v>
       </c>
-      <c r="V3" s="7">
+      <c r="V3" s="4">
         <v>319.69</v>
       </c>
-      <c r="W3" s="7">
+      <c r="W3" s="4">
         <v>6.2</v>
       </c>
-      <c r="X3" s="7">
+      <c r="X3" s="4">
         <v>5.59</v>
       </c>
-      <c r="Y3" s="7">
+      <c r="Y3" s="4">
         <v>4.93</v>
       </c>
-      <c r="Z3" s="7">
+      <c r="Z3" s="4">
         <v>14.53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" ht="20.25" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="4">
         <v>76.5</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="4">
         <v>3.5</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="4">
         <v>5.325</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="4">
         <v>6.5</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="4">
         <v>2.25</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="4">
         <v>4.5</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="4">
         <v>13.25</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="4">
         <v>2.75</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="5">
         <v>20</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="4">
         <v>6.97</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="4">
         <v>34.25</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="4">
         <v>24.75</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="4">
         <v>536.05</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="4">
         <v>37.33</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="4">
         <v>7.14</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="4">
         <v>5.2</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4" s="6">
         <v>2.51</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="4">
         <v>87.25</v>
       </c>
-      <c r="U4" s="7">
+      <c r="U4" s="4">
         <v>24.59</v>
       </c>
-      <c r="V4" s="7">
+      <c r="V4" s="4">
         <v>312.30999999999995</v>
       </c>
-      <c r="W4" s="7">
+      <c r="W4" s="4">
         <v>6.18</v>
       </c>
-      <c r="X4" s="7">
+      <c r="X4" s="4">
         <v>5.58</v>
       </c>
-      <c r="Y4" s="7">
+      <c r="Y4" s="4">
         <v>4.74</v>
       </c>
-      <c r="Z4" s="7">
+      <c r="Z4" s="4">
         <v>12.65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" ht="20.25" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="4">
         <v>62.75</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="4">
         <v>3.75</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="4">
         <v>6.225</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="4">
         <v>3.5</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="4">
         <v>1.75</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="4">
         <v>3.75</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="5">
         <v>9</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="4">
         <v>4.25</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="4">
         <v>28.5</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="4">
         <v>4.12</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="4">
         <v>59.75</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="4">
         <v>18.21</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="4">
         <v>446.4</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="4">
         <v>45.57</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="4">
         <v>9.59</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="4">
         <v>5.71</v>
       </c>
-      <c r="S5" s="9">
+      <c r="S5" s="6">
         <v>2.29</v>
       </c>
-      <c r="T5" s="7">
+      <c r="T5" s="4">
         <v>90.25</v>
       </c>
-      <c r="U5" s="7">
+      <c r="U5" s="4">
         <v>25.86</v>
       </c>
-      <c r="V5" s="7">
+      <c r="V5" s="4">
         <v>328.06</v>
       </c>
-      <c r="W5" s="7">
+      <c r="W5" s="4">
         <v>8.01</v>
       </c>
-      <c r="X5" s="7">
+      <c r="X5" s="4">
         <v>6.25</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="Y5" s="4">
         <v>4.93</v>
       </c>
-      <c r="Z5" s="7">
+      <c r="Z5" s="4">
         <v>21.92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" ht="20.25" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>61.5</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="4">
         <v>3.25</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="4">
         <v>4.5</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="4">
         <v>1.75</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="5">
         <v>1</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="4">
         <v>1.75</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="4">
         <v>4.5</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="4">
         <v>3.25</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="5">
         <v>16</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="4">
         <v>5.88</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="5">
         <v>29</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="4">
         <v>21.96</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="4">
         <v>474.91</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P6" s="4">
         <v>55.64</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="4">
         <v>11.01</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="4">
         <v>6.36</v>
       </c>
-      <c r="S6" s="9">
+      <c r="S6" s="6">
         <v>2.3</v>
       </c>
-      <c r="T6" s="7">
+      <c r="T6" s="4">
         <v>66.25</v>
       </c>
-      <c r="U6" s="8">
+      <c r="U6" s="5">
         <v>27.89</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="4">
         <v>309.08000000000004</v>
       </c>
-      <c r="W6" s="7">
+      <c r="W6" s="4">
         <v>8.94</v>
       </c>
-      <c r="X6" s="7">
+      <c r="X6" s="4">
         <v>7.37</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="Y6" s="4">
         <v>5.87</v>
       </c>
-      <c r="Z6" s="7">
+      <c r="Z6" s="4">
         <v>22.68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" ht="20.25" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>3</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="4">
         <v>49.25</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="5">
         <v>5</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="4">
         <v>5.225</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <v>3.25</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="4">
         <v>1.75</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="4">
         <v>2.5</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="4">
         <v>7.5</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="4">
         <v>2.75</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="5">
         <v>14</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="4">
         <v>5.12</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="5">
         <v>30</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="4">
         <v>24.165</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="4">
         <v>547.96</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="4">
         <v>49.63</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="4">
         <v>11.6</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="4">
         <v>6.78</v>
       </c>
-      <c r="S7" s="9">
+      <c r="S7" s="6">
         <v>2.2</v>
       </c>
-      <c r="T7" s="7">
+      <c r="T7" s="4">
         <v>55.5</v>
       </c>
-      <c r="U7" s="7">
+      <c r="U7" s="4">
         <v>27.87</v>
       </c>
-      <c r="V7" s="7">
+      <c r="V7" s="4">
         <v>246.7</v>
       </c>
-      <c r="W7" s="7">
+      <c r="W7" s="4">
         <v>9.11</v>
       </c>
-      <c r="X7" s="7">
+      <c r="X7" s="4">
         <v>7.24</v>
       </c>
-      <c r="Y7" s="7">
+      <c r="Y7" s="4">
         <v>5.95</v>
       </c>
-      <c r="Z7" s="7">
+      <c r="Z7" s="4">
         <v>22.51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" ht="20.25" customHeight="1">
+      <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="4">
         <v>90.75</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="4">
         <v>2.25</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="4">
         <v>5.35</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="4">
         <v>4.75</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="5">
         <v>2</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="4">
         <v>3.75</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="4">
         <v>10.5</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="4">
         <v>2.5</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="4">
         <v>21.5</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="4">
         <v>6.29</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="4">
         <v>44.5</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="4">
         <v>28.75</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="4">
         <v>705.7</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="4">
         <v>40.8</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="4">
         <v>9.31</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="4">
         <v>6.24</v>
       </c>
-      <c r="S8" s="9">
+      <c r="S8" s="6">
         <v>2.57</v>
       </c>
-      <c r="T8" s="8">
+      <c r="T8" s="5">
         <v>88</v>
       </c>
-      <c r="U8" s="7">
+      <c r="U8" s="4">
         <v>25.3</v>
       </c>
-      <c r="V8" s="7">
+      <c r="V8" s="4">
         <v>366.76</v>
       </c>
-      <c r="W8" s="7">
+      <c r="W8" s="4">
         <v>7.96</v>
       </c>
-      <c r="X8" s="7">
+      <c r="X8" s="4">
         <v>6.07</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="Y8" s="4">
         <v>4.75</v>
       </c>
-      <c r="Z8" s="7">
+      <c r="Z8" s="4">
         <v>15.61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" ht="20.25" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="4">
         <v>91.25</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="4">
         <v>1.5</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="4">
         <v>5.25</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="4">
         <v>4.75</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="4">
         <v>1.75</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="4">
         <v>3.25</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="4">
         <v>9.75</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="5">
         <v>3</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="4">
         <v>17.5</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="4">
         <v>5.98</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="4">
         <v>38.5</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="4">
         <v>19</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="4">
         <v>428.28</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9" s="4">
         <v>40.39</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="4">
         <v>8.99</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9" s="4">
         <v>5.22</v>
       </c>
-      <c r="S9" s="9">
+      <c r="S9" s="6">
         <v>2.55</v>
       </c>
-      <c r="T9" s="7">
+      <c r="T9" s="4">
         <v>98.75</v>
       </c>
-      <c r="U9" s="7">
+      <c r="U9" s="4">
         <v>21.89</v>
       </c>
-      <c r="V9" s="7">
+      <c r="V9" s="4">
         <v>260.12</v>
       </c>
-      <c r="W9" s="7">
+      <c r="W9" s="4">
         <v>7.37</v>
       </c>
-      <c r="X9" s="7">
+      <c r="X9" s="4">
         <v>5.42</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="Y9" s="4">
         <v>4.67</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="Z9" s="4">
         <v>13.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" ht="20.25" customHeight="1">
+      <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="3">
         <v>3</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="5">
         <v>84</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="4">
         <v>1.5</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="4">
         <v>6.449999999999999</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="4">
         <v>4.25</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="5">
         <v>2</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="4">
         <v>3.75</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="5">
         <v>10</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="4">
         <v>3.25</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="5">
         <v>24</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="4">
         <v>5.5</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="4">
         <v>37.5</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="4">
         <v>25.25</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="4">
         <v>599.37</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10" s="4">
         <v>41.75</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="4">
         <v>8.35</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="4">
         <v>5.41</v>
       </c>
-      <c r="S10" s="9">
+      <c r="S10" s="6">
         <v>2.23</v>
       </c>
-      <c r="T10" s="7">
+      <c r="T10" s="4">
         <v>80.5</v>
       </c>
-      <c r="U10" s="7">
+      <c r="U10" s="4">
         <v>28.04</v>
       </c>
-      <c r="V10" s="7">
+      <c r="V10" s="4">
         <v>272.98999999999995</v>
       </c>
-      <c r="W10" s="7">
+      <c r="W10" s="4">
         <v>6.19</v>
       </c>
-      <c r="X10" s="7">
+      <c r="X10" s="4">
         <v>6.13</v>
       </c>
-      <c r="Y10" s="7">
+      <c r="Y10" s="4">
         <v>4.6</v>
       </c>
-      <c r="Z10" s="7">
+      <c r="Z10" s="4">
         <v>12.31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" ht="20.25" customHeight="1">
+      <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="3">
         <v>1</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="4">
         <v>78.75</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="4">
         <v>0.75</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="4">
         <v>5.65</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="5">
         <v>5</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="4">
         <v>2.25</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="4">
         <v>4.75</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="5">
         <v>12</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="4">
         <v>4.5</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="4">
         <v>31.5</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="4">
         <v>5.9</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M11" s="5">
         <v>70</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="4">
         <v>22.83</v>
       </c>
-      <c r="O11" s="8">
+      <c r="O11" s="5">
         <v>554</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11" s="4">
         <v>36.42</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q11" s="4">
         <v>7.87</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11" s="4">
         <v>4.71</v>
       </c>
-      <c r="S11" s="9">
+      <c r="S11" s="6">
         <v>2.22</v>
       </c>
-      <c r="T11" s="7">
+      <c r="T11" s="4">
         <v>147.75</v>
       </c>
-      <c r="U11" s="7">
+      <c r="U11" s="4">
         <v>27.96</v>
       </c>
-      <c r="V11" s="7">
+      <c r="V11" s="4">
         <v>319.37000000000006</v>
       </c>
-      <c r="W11" s="7">
+      <c r="W11" s="4">
         <v>6.86</v>
       </c>
-      <c r="X11" s="7">
+      <c r="X11" s="4">
         <v>5.35</v>
       </c>
-      <c r="Y11" s="7">
+      <c r="Y11" s="4">
         <v>4.36</v>
       </c>
-      <c r="Z11" s="7">
+      <c r="Z11" s="4">
         <v>10.42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" ht="20.25" customHeight="1">
+      <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="4">
         <v>71.75</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="4">
         <v>0.5</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="4">
         <v>4.55</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="4">
         <v>4.75</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="4">
         <v>1.75</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="4">
         <v>3.5</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="5">
         <v>10</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="4">
         <v>3.75</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="5">
         <v>26</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="4">
         <v>5.7</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="4">
         <v>63.75</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="4">
         <v>21.42</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="4">
         <v>513.53</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="4">
         <v>34.71</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q12" s="4">
         <v>9.03</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="4">
         <v>5.07</v>
       </c>
-      <c r="S12" s="9">
+      <c r="S12" s="6">
         <v>2.38</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="4">
         <v>90.65</v>
       </c>
-      <c r="U12" s="7">
+      <c r="U12" s="4">
         <v>26.85</v>
       </c>
-      <c r="V12" s="7">
+      <c r="V12" s="4">
         <v>245.45999999999995</v>
       </c>
-      <c r="W12" s="7">
+      <c r="W12" s="4">
         <v>6.38</v>
       </c>
-      <c r="X12" s="7">
+      <c r="X12" s="4">
         <v>5.29</v>
       </c>
-      <c r="Y12" s="7">
+      <c r="Y12" s="4">
         <v>4.26</v>
       </c>
-      <c r="Z12" s="7">
+      <c r="Z12" s="4">
         <v>10.39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" ht="20.25" customHeight="1">
+      <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="3">
         <v>3</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="5">
         <v>83</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="4">
         <v>1.75</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="4">
         <v>6.075</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="5">
         <v>4</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="5">
         <v>2</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="5">
         <v>3</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="5">
         <v>9</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="4">
         <v>4.5</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="4">
         <v>29.75</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="4">
         <v>6.12</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="4">
         <v>66.5</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="4">
         <v>23.65</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="4">
         <v>426.84</v>
       </c>
-      <c r="P13" s="7">
+      <c r="P13" s="4">
         <v>32.54</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q13" s="4">
         <v>7.51</v>
       </c>
-      <c r="R13" s="7">
+      <c r="R13" s="4">
         <v>4.38</v>
       </c>
-      <c r="S13" s="9">
+      <c r="S13" s="6">
         <v>2.38</v>
       </c>
-      <c r="T13" s="7">
+      <c r="T13" s="4">
         <v>150.75</v>
       </c>
-      <c r="U13" s="7">
+      <c r="U13" s="4">
         <v>27.93</v>
       </c>
-      <c r="V13" s="7">
+      <c r="V13" s="4">
         <v>291.81</v>
       </c>
-      <c r="W13" s="7">
+      <c r="W13" s="4">
         <v>6.17</v>
       </c>
-      <c r="X13" s="7">
+      <c r="X13" s="4">
         <v>4.45</v>
       </c>
-      <c r="Y13" s="7">
+      <c r="Y13" s="4">
         <v>4.25</v>
       </c>
-      <c r="Z13" s="7">
+      <c r="Z13" s="4">
         <v>10.33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
-      <c r="A14" s="5" t="s">
+    <row r="14" ht="20.25" customHeight="1">
+      <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="5">
         <v>51</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="4">
         <v>2.5</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="4">
         <v>4.25</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="4">
         <v>3.5</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="4">
         <v>1.75</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="5">
         <v>3</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="4">
         <v>8.25</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="5">
         <v>3</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="4">
         <v>18.5</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="4">
         <v>5.88</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="4">
         <v>36.25</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="4">
         <v>24.7</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O14" s="4">
         <v>552.51</v>
       </c>
-      <c r="P14" s="7">
+      <c r="P14" s="4">
         <v>43.82</v>
       </c>
-      <c r="Q14" s="7">
+      <c r="Q14" s="4">
         <v>10.08</v>
       </c>
-      <c r="R14" s="7">
+      <c r="R14" s="4">
         <v>6.13</v>
       </c>
-      <c r="S14" s="9">
+      <c r="S14" s="6">
         <v>2.61</v>
       </c>
-      <c r="T14" s="7">
+      <c r="T14" s="4">
         <v>97.25</v>
       </c>
-      <c r="U14" s="7">
+      <c r="U14" s="4">
         <v>30.93</v>
       </c>
-      <c r="V14" s="7">
+      <c r="V14" s="4">
         <v>299.95000000000005</v>
       </c>
-      <c r="W14" s="7">
+      <c r="W14" s="4">
         <v>8.07</v>
       </c>
-      <c r="X14" s="7">
+      <c r="X14" s="4">
         <v>6.82</v>
       </c>
-      <c r="Y14" s="7">
+      <c r="Y14" s="4">
         <v>5.59</v>
       </c>
-      <c r="Z14" s="7">
+      <c r="Z14" s="4">
         <v>19.52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" ht="20.25" customHeight="1">
+      <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="5">
         <v>67</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="4">
         <v>1.5</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="5">
         <v>4</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="4">
         <v>2.5</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="4">
         <v>1.25</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="4">
         <v>1.5</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="4">
         <v>5.25</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="4">
         <v>3.25</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="5">
         <v>21</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="4">
         <v>6.73</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="4">
         <v>38.75</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="4">
         <v>26.62</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="4">
         <v>620.41</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="4">
         <v>46.89</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="Q15" s="4">
         <v>9.96</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R15" s="4">
         <v>6.02</v>
       </c>
-      <c r="S15" s="9">
+      <c r="S15" s="6">
         <v>2.47</v>
       </c>
-      <c r="T15" s="8">
+      <c r="T15" s="5">
         <v>99</v>
       </c>
-      <c r="U15" s="7">
+      <c r="U15" s="4">
         <v>32.49</v>
       </c>
-      <c r="V15" s="7">
+      <c r="V15" s="4">
         <v>405.84</v>
       </c>
-      <c r="W15" s="7">
+      <c r="W15" s="4">
         <v>7.52</v>
       </c>
-      <c r="X15" s="7">
+      <c r="X15" s="4">
         <v>6.67</v>
       </c>
-      <c r="Y15" s="7">
+      <c r="Y15" s="4">
         <v>5.63</v>
       </c>
-      <c r="Z15" s="7">
+      <c r="Z15" s="4">
         <v>18.15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
-      <c r="A16" s="5" t="s">
+    <row r="16" ht="20.25" customHeight="1">
+      <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="3">
         <v>3</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="4">
         <v>64.25</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="4">
         <v>0.75</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="4">
         <v>4.12</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="4">
         <v>2.75</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="5">
         <v>1</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="4">
         <v>1.25</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="5">
         <v>5</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="4">
         <v>3.25</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="5">
         <v>21</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="4">
         <v>6.61</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M16" s="5">
         <v>38</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="4">
         <v>24.7</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="4">
         <v>551.64</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16" s="4">
         <v>45.27</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="Q16" s="4">
         <v>10.15</v>
       </c>
-      <c r="R16" s="7">
+      <c r="R16" s="4">
         <v>5.45</v>
       </c>
-      <c r="S16" s="9">
+      <c r="S16" s="6">
         <v>2.5</v>
       </c>
-      <c r="T16" s="7">
+      <c r="T16" s="4">
         <v>100.25</v>
       </c>
-      <c r="U16" s="7">
+      <c r="U16" s="4">
         <v>31.74</v>
       </c>
-      <c r="V16" s="7">
+      <c r="V16" s="4">
         <v>358.57</v>
       </c>
-      <c r="W16" s="7">
+      <c r="W16" s="4">
         <v>7.45</v>
       </c>
-      <c r="X16" s="7">
+      <c r="X16" s="4">
         <v>6.59</v>
       </c>
-      <c r="Y16" s="7">
+      <c r="Y16" s="4">
         <v>5.41</v>
       </c>
-      <c r="Z16" s="7">
+      <c r="Z16" s="4">
         <v>18.32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" ht="20.25" customHeight="1">
+      <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="4">
         <v>92.5</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="4">
         <v>1.75</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="4">
         <v>6.199999999999999</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="4">
         <v>4.5</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="4">
         <v>2.25</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="4">
         <v>3.75</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="4">
         <v>10.5</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="4">
         <v>3.5</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="4">
         <v>26.5</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="4">
         <v>5.43</v>
       </c>
-      <c r="M17" s="8">
+      <c r="M17" s="5">
         <v>61</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N17" s="4">
         <v>45.75</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="4">
         <v>1035.12</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17" s="4">
         <v>44.13</v>
       </c>
-      <c r="Q17" s="7">
+      <c r="Q17" s="4">
         <v>9.53</v>
       </c>
-      <c r="R17" s="7">
+      <c r="R17" s="4">
         <v>6.41</v>
       </c>
-      <c r="S17" s="9">
+      <c r="S17" s="6">
         <v>2.47</v>
       </c>
-      <c r="T17" s="7">
+      <c r="T17" s="4">
         <v>126.75</v>
       </c>
-      <c r="U17" s="7">
+      <c r="U17" s="4">
         <v>19.04</v>
       </c>
-      <c r="V17" s="7">
+      <c r="V17" s="4">
         <v>455.61</v>
       </c>
-      <c r="W17" s="7">
+      <c r="W17" s="4">
         <v>8.17</v>
       </c>
-      <c r="X17" s="7">
+      <c r="X17" s="4">
         <v>6.79</v>
       </c>
-      <c r="Y17" s="7">
+      <c r="Y17" s="4">
         <v>5.37</v>
       </c>
-      <c r="Z17" s="7">
+      <c r="Z17" s="4">
         <v>20.21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" ht="20.25" customHeight="1">
+      <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="3">
         <v>2</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="5">
         <v>86</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="4">
         <v>2.5</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="4">
         <v>6.15</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="4">
         <v>5.25</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="4">
         <v>2.25</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="5">
         <v>4</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="4">
         <v>11.5</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="4">
         <v>4.75</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18" s="5">
         <v>24</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="4">
         <v>4.21</v>
       </c>
-      <c r="M18" s="8">
+      <c r="M18" s="5">
         <v>61</v>
       </c>
-      <c r="N18" s="7">
+      <c r="N18" s="4">
         <v>48</v>
       </c>
-      <c r="O18" s="7">
+      <c r="O18" s="4">
         <v>1005.94</v>
       </c>
-      <c r="P18" s="7">
+      <c r="P18" s="4">
         <v>49.84</v>
       </c>
-      <c r="Q18" s="7">
+      <c r="Q18" s="4">
         <v>10.45</v>
       </c>
-      <c r="R18" s="7">
+      <c r="R18" s="4">
         <v>7.13</v>
       </c>
-      <c r="S18" s="9">
+      <c r="S18" s="6">
         <v>2.22</v>
       </c>
-      <c r="T18" s="8">
+      <c r="T18" s="5">
         <v>136</v>
       </c>
-      <c r="U18" s="7">
+      <c r="U18" s="4">
         <v>21.91</v>
       </c>
-      <c r="V18" s="7">
+      <c r="V18" s="4">
         <v>427.13</v>
       </c>
-      <c r="W18" s="7">
+      <c r="W18" s="4">
         <v>8.3</v>
       </c>
-      <c r="X18" s="7">
+      <c r="X18" s="4">
         <v>6.87</v>
       </c>
-      <c r="Y18" s="7">
+      <c r="Y18" s="4">
         <v>5.68</v>
       </c>
-      <c r="Z18" s="7">
+      <c r="Z18" s="4">
         <v>22.76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" ht="20.25" customHeight="1">
+      <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="3">
         <v>3</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="4">
         <v>88.75</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="4">
         <v>2.5</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="4">
         <v>6.75</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="5">
         <v>4</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="5">
         <v>2</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="4">
         <v>3.5</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="4">
         <v>9.5</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="4">
         <v>5.45</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="4">
         <v>18.75</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="4">
         <v>5.22</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="4">
         <v>31.75</v>
       </c>
-      <c r="N19" s="7">
+      <c r="N19" s="4">
         <v>43</v>
       </c>
-      <c r="O19" s="7">
+      <c r="O19" s="4">
         <v>1005.39</v>
       </c>
-      <c r="P19" s="7">
+      <c r="P19" s="4">
         <v>48.4</v>
       </c>
-      <c r="Q19" s="7">
+      <c r="Q19" s="4">
         <v>8.89</v>
       </c>
-      <c r="R19" s="7">
+      <c r="R19" s="4">
         <v>6.21</v>
       </c>
-      <c r="S19" s="9">
+      <c r="S19" s="6">
         <v>2.41</v>
       </c>
-      <c r="T19" s="7">
+      <c r="T19" s="4">
         <v>134.52</v>
       </c>
-      <c r="U19" s="7">
+      <c r="U19" s="4">
         <v>20.56</v>
       </c>
-      <c r="V19" s="7">
+      <c r="V19" s="4">
         <v>476.83</v>
       </c>
-      <c r="W19" s="7">
+      <c r="W19" s="4">
         <v>8.35</v>
       </c>
-      <c r="X19" s="7">
+      <c r="X19" s="4">
         <v>6.22</v>
       </c>
-      <c r="Y19" s="7">
+      <c r="Y19" s="4">
         <v>5.54</v>
       </c>
-      <c r="Z19" s="7">
+      <c r="Z19" s="4">
         <v>20.51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
-      <c r="A20" s="5" t="s">
+    <row r="20" ht="20.25" customHeight="1">
+      <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="3">
         <v>1</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="4">
         <v>75.75</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="4">
         <v>3.25</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="4">
         <v>4.65</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="4">
         <v>7.25</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="4">
         <v>3.5</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="4">
         <v>5.25</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="5">
         <v>16</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="5">
         <v>4</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="4">
         <v>31.5</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="4">
         <v>7.77</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="4">
         <v>91.25</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="4">
         <v>26.69</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="4">
         <v>686.52</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P20" s="4">
         <v>33.34</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q20" s="4">
         <v>7.35</v>
       </c>
-      <c r="R20" s="7">
+      <c r="R20" s="4">
         <v>5.24</v>
       </c>
-      <c r="S20" s="9">
+      <c r="S20" s="6">
         <v>2.28</v>
       </c>
-      <c r="T20" s="8">
+      <c r="T20" s="5">
         <v>164</v>
       </c>
-      <c r="U20" s="7">
+      <c r="U20" s="4">
         <v>38.66</v>
       </c>
-      <c r="V20" s="7">
+      <c r="V20" s="4">
         <v>408.89</v>
       </c>
-      <c r="W20" s="7">
+      <c r="W20" s="4">
         <v>6.74</v>
       </c>
-      <c r="X20" s="7">
+      <c r="X20" s="4">
         <v>5.67</v>
       </c>
-      <c r="Y20" s="7">
+      <c r="Y20" s="4">
         <v>4.49</v>
       </c>
-      <c r="Z20" s="7">
+      <c r="Z20" s="4">
         <v>12.46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
-      <c r="A21" s="5" t="s">
+    <row r="21" ht="20.25" customHeight="1">
+      <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="3">
         <v>2</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="4">
         <v>58.75</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="4">
         <v>1.75</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="4">
         <v>4.15</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="4">
         <v>6.25</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="4">
         <v>2.75</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="4">
         <v>5.25</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="4">
         <v>14.25</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="5">
         <v>4</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21" s="5">
         <v>27</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="4">
         <v>6.37</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M21" s="4">
         <v>75.5</v>
       </c>
-      <c r="N21" s="7">
+      <c r="N21" s="4">
         <v>23.41</v>
       </c>
-      <c r="O21" s="7">
+      <c r="O21" s="4">
         <v>591.38</v>
       </c>
-      <c r="P21" s="7">
+      <c r="P21" s="4">
         <v>34.67</v>
       </c>
-      <c r="Q21" s="7">
+      <c r="Q21" s="4">
         <v>8.11</v>
       </c>
-      <c r="R21" s="7">
+      <c r="R21" s="4">
         <v>5.57</v>
       </c>
-      <c r="S21" s="9">
+      <c r="S21" s="6">
         <v>2.29</v>
       </c>
-      <c r="T21" s="8">
+      <c r="T21" s="5">
         <v>133</v>
       </c>
-      <c r="U21" s="7">
+      <c r="U21" s="4">
         <v>36.58</v>
       </c>
-      <c r="V21" s="7">
+      <c r="V21" s="4">
         <v>453.65</v>
       </c>
-      <c r="W21" s="7">
+      <c r="W21" s="4">
         <v>6.99</v>
       </c>
-      <c r="X21" s="7">
+      <c r="X21" s="4">
         <v>5.52</v>
       </c>
-      <c r="Y21" s="7">
+      <c r="Y21" s="4">
         <v>4.58</v>
       </c>
-      <c r="Z21" s="7">
+      <c r="Z21" s="4">
         <v>13.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
-      <c r="A22" s="5" t="s">
+    <row r="22" ht="20.25" customHeight="1">
+      <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="3">
         <v>3</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="4">
         <v>71.25</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="4">
         <v>2.25</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="4">
         <v>5.725</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="4">
         <v>6.25</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="4">
         <v>2.75</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="4">
         <v>3.5</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="4">
         <v>12.5</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="4">
         <v>4.75</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="4">
         <v>26.5</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="4">
         <v>6.27</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="4">
         <v>55.5</v>
       </c>
-      <c r="N22" s="7">
+      <c r="N22" s="4">
         <v>17.74</v>
       </c>
-      <c r="O22" s="7">
+      <c r="O22" s="4">
         <v>386.46</v>
       </c>
-      <c r="P22" s="7">
+      <c r="P22" s="4">
         <v>38.05</v>
       </c>
-      <c r="Q22" s="7">
+      <c r="Q22" s="4">
         <v>8.23</v>
       </c>
-      <c r="R22" s="8">
+      <c r="R22" s="5">
         <v>6</v>
       </c>
-      <c r="S22" s="9">
+      <c r="S22" s="6">
         <v>2.56</v>
       </c>
-      <c r="T22" s="7">
+      <c r="T22" s="4">
         <v>118.25</v>
       </c>
-      <c r="U22" s="7">
+      <c r="U22" s="4">
         <v>39.32</v>
       </c>
-      <c r="V22" s="7">
+      <c r="V22" s="4">
         <v>461.05</v>
       </c>
-      <c r="W22" s="7">
+      <c r="W22" s="4">
         <v>6.57</v>
       </c>
-      <c r="X22" s="7">
+      <c r="X22" s="4">
         <v>5.47</v>
       </c>
-      <c r="Y22" s="7">
+      <c r="Y22" s="4">
         <v>4.95</v>
       </c>
-      <c r="Z22" s="7">
+      <c r="Z22" s="4">
         <v>11.58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
-      <c r="A23" s="5" t="s">
+    <row r="23" ht="20.25" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="3">
         <v>1</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="4">
         <v>75.25</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="4">
         <v>3.25</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="4">
         <v>5.275</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="4">
         <v>5.25</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="4">
         <v>2.5</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="4">
         <v>4.5</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="4">
         <v>12.25</v>
       </c>
-      <c r="J23" s="7">
+      <c r="J23" s="4">
         <v>5.25</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K23" s="4">
         <v>27.5</v>
       </c>
-      <c r="L23" s="7">
+      <c r="L23" s="4">
         <v>7.04</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="4">
         <v>55.5</v>
       </c>
-      <c r="N23" s="7">
+      <c r="N23" s="4">
         <v>32.31</v>
       </c>
-      <c r="O23" s="7">
+      <c r="O23" s="4">
         <v>740.36</v>
       </c>
-      <c r="P23" s="7">
+      <c r="P23" s="4">
         <v>52.98</v>
       </c>
-      <c r="Q23" s="7">
+      <c r="Q23" s="4">
         <v>9.42</v>
       </c>
-      <c r="R23" s="7">
+      <c r="R23" s="4">
         <v>6.24</v>
       </c>
-      <c r="S23" s="9">
+      <c r="S23" s="6">
         <v>2.96</v>
       </c>
-      <c r="T23" s="7">
+      <c r="T23" s="4">
         <v>163.5</v>
       </c>
-      <c r="U23" s="7">
+      <c r="U23" s="4">
         <v>29.86</v>
       </c>
-      <c r="V23" s="7">
+      <c r="V23" s="4">
         <v>498.14000000000004</v>
       </c>
-      <c r="W23" s="7">
+      <c r="W23" s="4">
         <v>7.23</v>
       </c>
-      <c r="X23" s="7">
+      <c r="X23" s="4">
         <v>5.56</v>
       </c>
-      <c r="Y23" s="7">
+      <c r="Y23" s="4">
         <v>4.14</v>
       </c>
-      <c r="Z23" s="7">
+      <c r="Z23" s="4">
         <v>16.32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
-      <c r="A24" s="5" t="s">
+    <row r="24" ht="20.25" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="3">
         <v>2</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="4">
         <v>69.25</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="5">
         <v>2</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="4">
         <v>5.75</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="4">
         <v>3.5</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="4">
         <v>1.75</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="4">
         <v>2.75</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="5">
         <v>8</v>
       </c>
-      <c r="J24" s="8">
+      <c r="J24" s="5">
         <v>5</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="4">
         <v>26.25</v>
       </c>
-      <c r="L24" s="7">
+      <c r="L24" s="4">
         <v>6.34</v>
       </c>
-      <c r="M24" s="8">
+      <c r="M24" s="5">
         <v>52</v>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="4">
         <v>20.28</v>
       </c>
-      <c r="O24" s="7">
+      <c r="O24" s="4">
         <v>447.07</v>
       </c>
-      <c r="P24" s="7">
+      <c r="P24" s="4">
         <v>47.03</v>
       </c>
-      <c r="Q24" s="8">
+      <c r="Q24" s="5">
         <v>9</v>
       </c>
-      <c r="R24" s="7">
+      <c r="R24" s="4">
         <v>5.72</v>
       </c>
-      <c r="S24" s="9">
+      <c r="S24" s="6">
         <v>2.55</v>
       </c>
-      <c r="T24" s="7">
+      <c r="T24" s="4">
         <v>107.5</v>
       </c>
-      <c r="U24" s="7">
+      <c r="U24" s="4">
         <v>32.57</v>
       </c>
-      <c r="V24" s="7">
+      <c r="V24" s="4">
         <v>278.22999999999996</v>
       </c>
-      <c r="W24" s="7">
+      <c r="W24" s="4">
         <v>7.98</v>
       </c>
-      <c r="X24" s="7">
+      <c r="X24" s="4">
         <v>6.45</v>
       </c>
-      <c r="Y24" s="7">
+      <c r="Y24" s="4">
         <v>4.88</v>
       </c>
-      <c r="Z24" s="7">
+      <c r="Z24" s="4">
         <v>18.63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" ht="20.25" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="3">
         <v>3</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="4">
         <v>53.25</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="4">
         <v>3.5</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="4">
         <v>4.675</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="4">
         <v>3.5</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="5">
         <v>2</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="4">
         <v>3.5</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="5">
         <v>9</v>
       </c>
-      <c r="J25" s="7">
+      <c r="J25" s="4">
         <v>3.25</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25" s="5">
         <v>22</v>
       </c>
-      <c r="L25" s="7">
+      <c r="L25" s="4">
         <v>7.9</v>
       </c>
-      <c r="M25" s="8">
+      <c r="M25" s="5">
         <v>42</v>
       </c>
-      <c r="N25" s="7">
+      <c r="N25" s="4">
         <v>19.33</v>
       </c>
-      <c r="O25" s="7">
+      <c r="O25" s="4">
         <v>446.7</v>
       </c>
-      <c r="P25" s="7">
+      <c r="P25" s="4">
         <v>51.59</v>
       </c>
-      <c r="Q25" s="7">
+      <c r="Q25" s="4">
         <v>9.38</v>
       </c>
-      <c r="R25" s="7">
+      <c r="R25" s="4">
         <v>6.43</v>
       </c>
-      <c r="S25" s="9">
+      <c r="S25" s="6">
         <v>2.46</v>
       </c>
-      <c r="T25" s="7">
+      <c r="T25" s="4">
         <v>102.5</v>
       </c>
-      <c r="U25" s="7">
+      <c r="U25" s="4">
         <v>34.53</v>
       </c>
-      <c r="V25" s="7">
+      <c r="V25" s="4">
         <v>304.15000000000003</v>
       </c>
-      <c r="W25" s="7">
+      <c r="W25" s="4">
         <v>8.34</v>
       </c>
-      <c r="X25" s="7">
+      <c r="X25" s="4">
         <v>6.73</v>
       </c>
-      <c r="Y25" s="7">
+      <c r="Y25" s="4">
         <v>5.28</v>
       </c>
-      <c r="Z25" s="7">
+      <c r="Z25" s="4">
         <v>17.44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" ht="20.25" customHeight="1">
+      <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="3">
         <v>1</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="5">
         <v>77</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="4">
         <v>2.5</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="4">
         <v>5.625</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="4">
         <v>4.25</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="4">
         <v>1.75</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="5">
         <v>4</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I26" s="5">
         <v>10</v>
       </c>
-      <c r="J26" s="7">
+      <c r="J26" s="4">
         <v>3.5</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K26" s="5">
         <v>21</v>
       </c>
-      <c r="L26" s="7">
+      <c r="L26" s="4">
         <v>5.31</v>
       </c>
-      <c r="M26" s="8">
+      <c r="M26" s="5">
         <v>29</v>
       </c>
-      <c r="N26" s="7">
+      <c r="N26" s="4">
         <v>15.75</v>
       </c>
-      <c r="O26" s="7">
+      <c r="O26" s="4">
         <v>442.75</v>
       </c>
-      <c r="P26" s="7">
+      <c r="P26" s="4">
         <v>35.28</v>
       </c>
-      <c r="Q26" s="7">
+      <c r="Q26" s="4">
         <v>6.71</v>
       </c>
-      <c r="R26" s="7">
+      <c r="R26" s="4">
         <v>4.08</v>
       </c>
-      <c r="S26" s="9">
+      <c r="S26" s="6">
         <v>2.7</v>
       </c>
-      <c r="T26" s="7">
+      <c r="T26" s="4">
         <v>76.75</v>
       </c>
-      <c r="U26" s="7">
+      <c r="U26" s="4">
         <v>15.53</v>
       </c>
-      <c r="V26" s="7">
+      <c r="V26" s="4">
         <v>230.16999999999996</v>
       </c>
-      <c r="W26" s="7">
+      <c r="W26" s="4">
         <v>6.33</v>
       </c>
-      <c r="X26" s="7">
+      <c r="X26" s="4">
         <v>4.87</v>
       </c>
-      <c r="Y26" s="8">
+      <c r="Y26" s="5">
         <v>4</v>
       </c>
-      <c r="Z26" s="7">
+      <c r="Z26" s="4">
         <v>12.45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
-      <c r="A27" s="5" t="s">
+    <row r="27" ht="20.25" customHeight="1">
+      <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="3">
         <v>2</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="4">
         <v>64.75</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="4">
         <v>3.15</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="4">
         <v>6.375</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="5">
         <v>5</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="5">
         <v>2</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="5">
         <v>4</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I27" s="5">
         <v>11</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="4">
         <v>3.25</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="4">
         <v>22.75</v>
       </c>
-      <c r="L27" s="7">
+      <c r="L27" s="4">
         <v>5.87</v>
       </c>
-      <c r="M27" s="7">
+      <c r="M27" s="4">
         <v>39.25</v>
       </c>
-      <c r="N27" s="7">
+      <c r="N27" s="4">
         <v>24.75</v>
       </c>
-      <c r="O27" s="7">
+      <c r="O27" s="4">
         <v>540.28</v>
       </c>
-      <c r="P27" s="7">
+      <c r="P27" s="4">
         <v>35.36</v>
       </c>
-      <c r="Q27" s="7">
+      <c r="Q27" s="4">
         <v>6.48</v>
       </c>
-      <c r="R27" s="7">
+      <c r="R27" s="4">
         <v>4.45</v>
       </c>
-      <c r="S27" s="9">
+      <c r="S27" s="6">
         <v>2.94</v>
       </c>
-      <c r="T27" s="7">
+      <c r="T27" s="4">
         <v>84.25</v>
       </c>
-      <c r="U27" s="7">
+      <c r="U27" s="4">
         <v>17.12</v>
       </c>
-      <c r="V27" s="7">
+      <c r="V27" s="4">
         <v>287.7</v>
       </c>
-      <c r="W27" s="7">
+      <c r="W27" s="4">
         <v>6.26</v>
       </c>
-      <c r="X27" s="7">
+      <c r="X27" s="4">
         <v>5.05</v>
       </c>
-      <c r="Y27" s="7">
+      <c r="Y27" s="4">
         <v>4.82</v>
       </c>
-      <c r="Z27" s="7">
+      <c r="Z27" s="4">
         <v>13.87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25">
-      <c r="A28" s="5" t="s">
+    <row r="28" ht="20.25" customHeight="1">
+      <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="3">
         <v>3</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="4">
         <v>80.25</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="4">
         <v>3.5</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="4">
         <v>6.425000000000001</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="4">
         <v>7.25</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="4">
         <v>3.25</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="4">
         <v>6.75</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="4">
         <v>17.25</v>
       </c>
-      <c r="J28" s="8">
+      <c r="J28" s="5">
         <v>4</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K28" s="4">
         <v>25.5</v>
       </c>
-      <c r="L28" s="7">
+      <c r="L28" s="4">
         <v>5.4</v>
       </c>
-      <c r="M28" s="8">
+      <c r="M28" s="5">
         <v>45</v>
       </c>
-      <c r="N28" s="7">
+      <c r="N28" s="4">
         <v>32</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O28" s="4">
         <v>627.94</v>
       </c>
-      <c r="P28" s="7">
+      <c r="P28" s="4">
         <v>42.96</v>
       </c>
-      <c r="Q28" s="7">
+      <c r="Q28" s="4">
         <v>8.69</v>
       </c>
-      <c r="R28" s="7">
+      <c r="R28" s="4">
         <v>5.23</v>
       </c>
-      <c r="S28" s="9">
+      <c r="S28" s="6">
         <v>2.44</v>
       </c>
-      <c r="T28" s="7">
+      <c r="T28" s="4">
         <v>88.4</v>
       </c>
-      <c r="U28" s="7">
+      <c r="U28" s="4">
         <v>12.85</v>
       </c>
-      <c r="V28" s="7">
+      <c r="V28" s="4">
         <v>291.09</v>
       </c>
-      <c r="W28" s="7">
+      <c r="W28" s="4">
         <v>6.93</v>
       </c>
-      <c r="X28" s="7">
+      <c r="X28" s="4">
         <v>5.43</v>
       </c>
-      <c r="Y28" s="7">
+      <c r="Y28" s="4">
         <v>4.27</v>
       </c>
-      <c r="Z28" s="7">
+      <c r="Z28" s="4">
         <v>13.59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25">
-      <c r="A29" s="5" t="s">
+    <row r="29" ht="20.25" customHeight="1">
+      <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="5">
         <v>76</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="5">
         <v>2</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="4">
         <v>5.45</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="4">
         <v>4.25</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="4">
         <v>1.75</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="4">
         <v>2.25</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="4">
         <v>8.25</v>
       </c>
-      <c r="J29" s="7">
+      <c r="J29" s="4">
         <v>2.75</v>
       </c>
-      <c r="K29" s="7">
+      <c r="K29" s="4">
         <v>16.25</v>
       </c>
-      <c r="L29" s="7">
+      <c r="L29" s="4">
         <v>5.29</v>
       </c>
-      <c r="M29" s="8">
+      <c r="M29" s="5">
         <v>37</v>
       </c>
-      <c r="N29" s="7">
+      <c r="N29" s="4">
         <v>31.25</v>
       </c>
-      <c r="O29" s="7">
+      <c r="O29" s="4">
         <v>432.87</v>
       </c>
-      <c r="P29" s="7">
+      <c r="P29" s="4">
         <v>44.46</v>
       </c>
-      <c r="Q29" s="7">
+      <c r="Q29" s="4">
         <v>8.86</v>
       </c>
-      <c r="R29" s="7">
+      <c r="R29" s="4">
         <v>6.3</v>
       </c>
-      <c r="S29" s="9">
+      <c r="S29" s="6">
         <v>3</v>
       </c>
-      <c r="T29" s="7">
+      <c r="T29" s="4">
         <v>82.75</v>
       </c>
-      <c r="U29" s="7">
+      <c r="U29" s="4">
         <v>31.46</v>
       </c>
-      <c r="V29" s="7">
+      <c r="V29" s="4">
         <v>283.14</v>
       </c>
-      <c r="W29" s="7">
+      <c r="W29" s="4">
         <v>6.86</v>
       </c>
-      <c r="X29" s="7">
+      <c r="X29" s="4">
         <v>5.87</v>
       </c>
-      <c r="Y29" s="7">
+      <c r="Y29" s="4">
         <v>4.92</v>
       </c>
-      <c r="Z29" s="7">
+      <c r="Z29" s="4">
         <v>17.54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.25">
-      <c r="A30" s="5" t="s">
+    <row r="30" ht="20.25" customHeight="1">
+      <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="3">
         <v>2</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="4">
         <v>82.5</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="4">
         <v>2.5</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="4">
         <v>4.125</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="4">
         <v>2.25</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="4">
         <v>1.25</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="4">
         <v>2.5</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I30" s="5">
         <v>6</v>
       </c>
-      <c r="J30" s="7">
+      <c r="J30" s="4">
         <v>1.5</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="4">
         <v>21.5</v>
       </c>
-      <c r="L30" s="7">
+      <c r="L30" s="4">
         <v>4.76</v>
       </c>
-      <c r="M30" s="8">
+      <c r="M30" s="5">
         <v>32</v>
       </c>
-      <c r="N30" s="7">
+      <c r="N30" s="4">
         <v>19.39</v>
       </c>
-      <c r="O30" s="7">
+      <c r="O30" s="4">
         <v>444.46</v>
       </c>
-      <c r="P30" s="7">
+      <c r="P30" s="4">
         <v>45.76</v>
       </c>
-      <c r="Q30" s="7">
+      <c r="Q30" s="4">
         <v>9.75</v>
       </c>
-      <c r="R30" s="7">
+      <c r="R30" s="4">
         <v>6.19</v>
       </c>
-      <c r="S30" s="9">
+      <c r="S30" s="6">
         <v>2.93</v>
       </c>
-      <c r="T30" s="7">
+      <c r="T30" s="4">
         <v>91.5</v>
       </c>
-      <c r="U30" s="7">
+      <c r="U30" s="4">
         <v>28.79</v>
       </c>
-      <c r="V30" s="7">
+      <c r="V30" s="4">
         <v>292.2100000000001</v>
       </c>
-      <c r="W30" s="7">
+      <c r="W30" s="4">
         <v>7.22</v>
       </c>
-      <c r="X30" s="7">
+      <c r="X30" s="4">
         <v>6.23</v>
       </c>
-      <c r="Y30" s="7">
+      <c r="Y30" s="4">
         <v>5.21</v>
       </c>
-      <c r="Z30" s="7">
+      <c r="Z30" s="4">
         <v>16.45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25">
-      <c r="A31" s="5" t="s">
+    <row r="31" ht="20.25" customHeight="1">
+      <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="3">
         <v>3</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="4">
         <v>85.75</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="4">
         <v>3.75</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="4">
         <v>4.35</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="5">
         <v>3</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="4">
         <v>1.5</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="4">
         <v>2.5</v>
       </c>
-      <c r="I31" s="8">
+      <c r="I31" s="5">
         <v>7</v>
       </c>
-      <c r="J31" s="7">
+      <c r="J31" s="4">
         <v>2.25</v>
       </c>
-      <c r="K31" s="7">
+      <c r="K31" s="4">
         <v>17.5</v>
       </c>
-      <c r="L31" s="7">
+      <c r="L31" s="4">
         <v>6.22</v>
       </c>
-      <c r="M31" s="7">
+      <c r="M31" s="4">
         <v>29.5</v>
       </c>
-      <c r="N31" s="7">
+      <c r="N31" s="4">
         <v>22.14</v>
       </c>
-      <c r="O31" s="7">
+      <c r="O31" s="4">
         <v>459.92</v>
       </c>
-      <c r="P31" s="7">
+      <c r="P31" s="4">
         <v>49.45</v>
       </c>
-      <c r="Q31" s="7">
+      <c r="Q31" s="4">
         <v>8.93</v>
       </c>
-      <c r="R31" s="7">
+      <c r="R31" s="4">
         <v>5.85</v>
       </c>
-      <c r="S31" s="9">
+      <c r="S31" s="6">
         <v>3.1</v>
       </c>
-      <c r="T31" s="8">
+      <c r="T31" s="5">
         <v>83</v>
       </c>
-      <c r="U31" s="7">
+      <c r="U31" s="4">
         <v>29.93</v>
       </c>
-      <c r="V31" s="7">
+      <c r="V31" s="4">
         <v>304.91</v>
       </c>
-      <c r="W31" s="7">
+      <c r="W31" s="4">
         <v>7.95</v>
       </c>
-      <c r="X31" s="7">
+      <c r="X31" s="4">
         <v>6.57</v>
       </c>
-      <c r="Y31" s="7">
+      <c r="Y31" s="4">
         <v>5.72</v>
       </c>
-      <c r="Z31" s="7">
+      <c r="Z31" s="4">
         <v>18.43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.25">
-      <c r="A32" s="5" t="s">
+    <row r="32" ht="20.25" customHeight="1">
+      <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="3">
         <v>1</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="4">
         <v>79.25</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="4">
         <v>2.5</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="4">
         <v>6.575</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="4">
         <v>4.5</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="5">
         <v>2</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="4">
         <v>3.5</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I32" s="5">
         <v>10</v>
       </c>
-      <c r="J32" s="7">
+      <c r="J32" s="4">
         <v>4.75</v>
       </c>
-      <c r="K32" s="7">
+      <c r="K32" s="4">
         <v>22.5</v>
       </c>
-      <c r="L32" s="7">
+      <c r="L32" s="4">
         <v>6.4</v>
       </c>
-      <c r="M32" s="7">
+      <c r="M32" s="4">
         <v>52.75</v>
       </c>
-      <c r="N32" s="7">
+      <c r="N32" s="4">
         <v>19.43</v>
       </c>
-      <c r="O32" s="7">
+      <c r="O32" s="4">
         <v>443.71</v>
       </c>
-      <c r="P32" s="7">
+      <c r="P32" s="4">
         <v>44.81</v>
       </c>
-      <c r="Q32" s="7">
+      <c r="Q32" s="4">
         <v>9.71</v>
       </c>
-      <c r="R32" s="7">
+      <c r="R32" s="4">
         <v>4.34</v>
       </c>
-      <c r="S32" s="9">
+      <c r="S32" s="6">
         <v>2.85</v>
       </c>
-      <c r="T32" s="7">
+      <c r="T32" s="4">
         <v>93.45</v>
       </c>
-      <c r="U32" s="7">
+      <c r="U32" s="4">
         <v>35.05</v>
       </c>
-      <c r="V32" s="7">
+      <c r="V32" s="4">
         <v>320.8700000000001</v>
       </c>
-      <c r="W32" s="7">
+      <c r="W32" s="4">
         <v>7.21</v>
       </c>
-      <c r="X32" s="7">
+      <c r="X32" s="4">
         <v>6.01</v>
       </c>
-      <c r="Y32" s="7">
+      <c r="Y32" s="4">
         <v>4.23</v>
       </c>
-      <c r="Z32" s="7">
+      <c r="Z32" s="4">
         <v>14.24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.25">
-      <c r="A33" s="5" t="s">
+    <row r="33" ht="20.25" customHeight="1">
+      <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="3">
         <v>2</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="4">
         <v>67.75</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="4">
         <v>3.75</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="4">
         <v>6.3</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="4">
         <v>4.75</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="5">
         <v>4</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="4">
         <v>3.75</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="4">
         <v>12.5</v>
       </c>
-      <c r="J33" s="8">
+      <c r="J33" s="5">
         <v>5</v>
       </c>
-      <c r="K33" s="7">
+      <c r="K33" s="4">
         <v>22.5</v>
       </c>
-      <c r="L33" s="7">
+      <c r="L33" s="4">
         <v>6.62</v>
       </c>
-      <c r="M33" s="7">
+      <c r="M33" s="4">
         <v>51.25</v>
       </c>
-      <c r="N33" s="7">
+      <c r="N33" s="4">
         <v>13.6</v>
       </c>
-      <c r="O33" s="7">
+      <c r="O33" s="4">
         <v>320.19</v>
       </c>
-      <c r="P33" s="7">
+      <c r="P33" s="4">
         <v>43.43</v>
       </c>
-      <c r="Q33" s="7">
+      <c r="Q33" s="4">
         <v>9.03</v>
       </c>
-      <c r="R33" s="7">
+      <c r="R33" s="4">
         <v>5.23</v>
       </c>
-      <c r="S33" s="9">
+      <c r="S33" s="6">
         <v>2.69</v>
       </c>
-      <c r="T33" s="7">
+      <c r="T33" s="4">
         <v>107.5</v>
       </c>
-      <c r="U33" s="7">
+      <c r="U33" s="4">
         <v>31.72</v>
       </c>
-      <c r="V33" s="7">
+      <c r="V33" s="4">
         <v>274.03</v>
       </c>
-      <c r="W33" s="7">
+      <c r="W33" s="4">
         <v>7.3</v>
       </c>
-      <c r="X33" s="7">
+      <c r="X33" s="4">
         <v>5.87</v>
       </c>
-      <c r="Y33" s="7">
+      <c r="Y33" s="4">
         <v>4.79</v>
       </c>
-      <c r="Z33" s="7">
+      <c r="Z33" s="4">
         <v>15.13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="20.25">
-      <c r="A34" s="5" t="s">
+    <row r="34" ht="20.25" customHeight="1">
+      <c r="A34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="3">
         <v>3</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="5">
         <v>79</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="4">
         <v>3.25</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="4">
         <v>5.65</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="5">
         <v>4</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="4">
         <v>2.25</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34" s="5">
         <v>3</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="4">
         <v>9.25</v>
       </c>
-      <c r="J34" s="7">
+      <c r="J34" s="4">
         <v>4.25</v>
       </c>
-      <c r="K34" s="7">
+      <c r="K34" s="4">
         <v>26.75</v>
       </c>
-      <c r="L34" s="7">
+      <c r="L34" s="4">
         <v>6.21</v>
       </c>
-      <c r="M34" s="8">
+      <c r="M34" s="5">
         <v>51</v>
       </c>
-      <c r="N34" s="7">
+      <c r="N34" s="4">
         <v>24.21</v>
       </c>
-      <c r="O34" s="7">
+      <c r="O34" s="4">
         <v>470.23</v>
       </c>
-      <c r="P34" s="7">
+      <c r="P34" s="4">
         <v>43.9</v>
       </c>
-      <c r="Q34" s="7">
+      <c r="Q34" s="4">
         <v>8.79</v>
       </c>
-      <c r="R34" s="7">
+      <c r="R34" s="4">
         <v>5.02</v>
       </c>
-      <c r="S34" s="9">
+      <c r="S34" s="6">
         <v>2.74</v>
       </c>
-      <c r="T34" s="7">
+      <c r="T34" s="4">
         <v>97.54</v>
       </c>
-      <c r="U34" s="7">
+      <c r="U34" s="4">
         <v>38.85</v>
       </c>
-      <c r="V34" s="7">
+      <c r="V34" s="4">
         <v>196.07</v>
       </c>
-      <c r="W34" s="7">
+      <c r="W34" s="4">
         <v>7.26</v>
       </c>
-      <c r="X34" s="7">
+      <c r="X34" s="4">
         <v>5.68</v>
       </c>
-      <c r="Y34" s="7">
+      <c r="Y34" s="4">
         <v>4.52</v>
       </c>
-      <c r="Z34" s="7">
+      <c r="Z34" s="4">
         <v>14.27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25">
-      <c r="A35" s="5" t="s">
+    <row r="35" ht="20.25" customHeight="1">
+      <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="3">
         <v>1</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="5">
         <v>85</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="4">
         <v>0.75</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="4">
         <v>6.750000000000001</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="5">
         <v>3</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="4">
         <v>1.5</v>
       </c>
-      <c r="H35" s="7">
+      <c r="H35" s="4">
         <v>2.25</v>
       </c>
-      <c r="I35" s="7">
+      <c r="I35" s="4">
         <v>6.75</v>
       </c>
-      <c r="J35" s="7">
+      <c r="J35" s="4">
         <v>4.5</v>
       </c>
-      <c r="K35" s="7">
+      <c r="K35" s="4">
         <v>26.75</v>
       </c>
-      <c r="L35" s="7">
+      <c r="L35" s="4">
         <v>7.62</v>
       </c>
-      <c r="M35" s="7">
+      <c r="M35" s="4">
         <v>83.75</v>
       </c>
-      <c r="N35" s="7">
+      <c r="N35" s="4">
         <v>19.98</v>
       </c>
-      <c r="O35" s="7">
+      <c r="O35" s="4">
         <v>443.79</v>
       </c>
-      <c r="P35" s="8">
+      <c r="P35" s="5">
         <v>40</v>
       </c>
-      <c r="Q35" s="7">
+      <c r="Q35" s="4">
         <v>8.67</v>
       </c>
-      <c r="R35" s="7">
+      <c r="R35" s="4">
         <v>5.22</v>
       </c>
-      <c r="S35" s="9">
+      <c r="S35" s="6">
         <v>2.37</v>
       </c>
-      <c r="T35" s="7">
+      <c r="T35" s="4">
         <v>103.4</v>
       </c>
-      <c r="U35" s="7">
+      <c r="U35" s="4">
         <v>29.48</v>
       </c>
-      <c r="V35" s="7">
+      <c r="V35" s="4">
         <v>391.0099999999999</v>
       </c>
-      <c r="W35" s="7">
+      <c r="W35" s="4">
         <v>7.06</v>
       </c>
-      <c r="X35" s="7">
+      <c r="X35" s="4">
         <v>5.24</v>
       </c>
-      <c r="Y35" s="7">
+      <c r="Y35" s="4">
         <v>4.55</v>
       </c>
-      <c r="Z35" s="7">
+      <c r="Z35" s="4">
         <v>11.94</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="20.25">
-      <c r="A36" s="5" t="s">
+    <row r="36" ht="20.25" customHeight="1">
+      <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="3">
         <v>2</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="4">
         <v>62.25</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="4">
         <v>1.5</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="4">
         <v>5.525</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="5">
         <v>6</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="4">
         <v>2.75</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="5">
         <v>5</v>
       </c>
-      <c r="I36" s="7">
+      <c r="I36" s="4">
         <v>13.75</v>
       </c>
-      <c r="J36" s="7">
+      <c r="J36" s="4">
         <v>4.25</v>
       </c>
-      <c r="K36" s="7">
+      <c r="K36" s="4">
         <v>24.75</v>
       </c>
-      <c r="L36" s="7">
+      <c r="L36" s="4">
         <v>5.97</v>
       </c>
-      <c r="M36" s="7">
+      <c r="M36" s="4">
         <v>63.25</v>
       </c>
-      <c r="N36" s="7">
+      <c r="N36" s="4">
         <v>28.92</v>
       </c>
-      <c r="O36" s="7">
+      <c r="O36" s="4">
         <v>428.65</v>
       </c>
-      <c r="P36" s="7">
+      <c r="P36" s="4">
         <v>41.23</v>
       </c>
-      <c r="Q36" s="7">
+      <c r="Q36" s="4">
         <v>7.84</v>
       </c>
-      <c r="R36" s="7">
+      <c r="R36" s="4">
         <v>5.25</v>
       </c>
-      <c r="S36" s="9">
+      <c r="S36" s="6">
         <v>2.21</v>
       </c>
-      <c r="T36" s="7">
+      <c r="T36" s="4">
         <v>93.15</v>
       </c>
-      <c r="U36" s="7">
+      <c r="U36" s="4">
         <v>29.78</v>
       </c>
-      <c r="V36" s="7">
+      <c r="V36" s="4">
         <v>287.65</v>
       </c>
-      <c r="W36" s="7">
+      <c r="W36" s="4">
         <v>6.75</v>
       </c>
-      <c r="X36" s="7">
+      <c r="X36" s="4">
         <v>5.13</v>
       </c>
-      <c r="Y36" s="7">
+      <c r="Y36" s="4">
         <v>4.22</v>
       </c>
-      <c r="Z36" s="7">
+      <c r="Z36" s="4">
         <v>12.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25">
-      <c r="A37" s="5" t="s">
+    <row r="37" ht="20.25" customHeight="1">
+      <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="3">
         <v>3</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="4">
         <v>82.5</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="4">
         <v>0.75</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="4">
         <v>5.875</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="4">
         <v>4.75</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="4">
         <v>2.5</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="4">
         <v>4.75</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="5">
         <v>12</v>
       </c>
-      <c r="J37" s="7">
+      <c r="J37" s="4">
         <v>4.5</v>
       </c>
-      <c r="K37" s="7">
+      <c r="K37" s="4">
         <v>23.75</v>
       </c>
-      <c r="L37" s="7">
+      <c r="L37" s="4">
         <v>6.41</v>
       </c>
-      <c r="M37" s="7">
+      <c r="M37" s="4">
         <v>58.25</v>
       </c>
-      <c r="N37" s="7">
+      <c r="N37" s="4">
         <v>27</v>
       </c>
-      <c r="O37" s="7">
+      <c r="O37" s="4">
         <v>412.43</v>
       </c>
-      <c r="P37" s="7">
+      <c r="P37" s="4">
         <v>42.4</v>
       </c>
-      <c r="Q37" s="7">
+      <c r="Q37" s="4">
         <v>8.02</v>
       </c>
-      <c r="R37" s="7">
+      <c r="R37" s="4">
         <v>5.75</v>
       </c>
-      <c r="S37" s="9">
+      <c r="S37" s="6">
         <v>2.14</v>
       </c>
-      <c r="T37" s="7">
+      <c r="T37" s="4">
         <v>98.45</v>
       </c>
-      <c r="U37" s="7">
+      <c r="U37" s="4">
         <v>29.92</v>
       </c>
-      <c r="V37" s="7">
+      <c r="V37" s="4">
         <v>322.61</v>
       </c>
-      <c r="W37" s="7">
+      <c r="W37" s="4">
         <v>7.12</v>
       </c>
-      <c r="X37" s="7">
+      <c r="X37" s="4">
         <v>4.87</v>
       </c>
-      <c r="Y37" s="7">
+      <c r="Y37" s="4">
         <v>4.13</v>
       </c>
-      <c r="Z37" s="7">
+      <c r="Z37" s="4">
         <v>11.55</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:Z37"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>